<commit_message>
Changing how Nan is handled to fix potential null value issue and removing autoincrement flag on survey seems to help
</commit_message>
<xml_diff>
--- a/Lookups.xlsx
+++ b/Lookups.xlsx
@@ -447,7 +447,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <sheetData/>
-  <pageMargins top="1" right="0.75" left="0.75" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins top="1" bottom="1" header="0.5" footer="0.5" right="0.75" left="0.75"/>
 </worksheet>
 </file>
 
@@ -682,6 +682,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" right="0.75" left="0.75" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins top="1" bottom="1" header="0.5" footer="0.5" right="0.75" left="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor changes so that all tests pass
</commit_message>
<xml_diff>
--- a/Lookups.xlsx
+++ b/Lookups.xlsx
@@ -437,32 +437,32 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins top="1" bottom="1" header="0.5" footer="0.5" right="0.75" left="0.75"/>
+  <pageMargins top="1" footer="0.5" right="0.75" left="0.75" header="0.5" bottom="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row spans="1:24" r="1">
       <c t="s" r="A1">
@@ -682,6 +682,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" bottom="1" header="0.5" footer="0.5" right="0.75" left="0.75"/>
+  <pageMargins top="1" footer="0.5" right="0.75" left="0.75" header="0.5" bottom="1"/>
 </worksheet>
 </file>
</xml_diff>